<commit_message>
BurnUp updated and SprintProtokol 4 Added
</commit_message>
<xml_diff>
--- a/Documentation/Burn-Up_Chart.xlsx
+++ b/Documentation/Burn-Up_Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matus\Documents\ITP2_PC\ITP2_PC_Game\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wiede\Documents\ITP2_PC_Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FB3C85A-19DD-4CB5-AAB2-EFD5CF11EAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F50AFC-5768-4398-9476-1CFC12F97BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28005" windowHeight="16440" xr2:uid="{7FB4506B-606D-4E3C-8334-B76E2DC527AB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{7FB4506B-606D-4E3C-8334-B76E2DC527AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -450,6 +449,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>165</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1903,17 +1908,17 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1927,7 +1932,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1941,7 +1946,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <f>SUM(A2+1)</f>
         <v>2</v>
@@ -1957,23 +1962,23 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A26" si="0">SUM(A3+1)</f>
+        <f t="shared" ref="A4:A13" si="0">SUM(A3+1)</f>
         <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>300</v>
       </c>
       <c r="C4" s="2">
-        <f t="shared" ref="C4:C13" si="1">C3+D4</f>
+        <f t="shared" ref="C4:C9" si="1">C3+D4</f>
         <v>68</v>
       </c>
       <c r="D4">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1989,7 +1994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2005,7 +2010,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2021,7 +2026,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2029,9 +2034,15 @@
       <c r="B8" s="2">
         <v>300</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="D8">
+        <v>27</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2039,9 +2050,15 @@
       <c r="B9" s="2">
         <v>300</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2051,7 +2068,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2061,7 +2078,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2071,7 +2088,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>

</xml_diff>